<commit_message>
[excel-pipeline] hash_id:b8be579 commit_msg:修改装备数值 ...
</commit_message>
<xml_diff>
--- a/config/excel/EquipEnchant.xlsx
+++ b/config/excel/EquipEnchant.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29560" windowHeight="17020"/>
+    <workbookView windowWidth="28125" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="EquipEnchant" sheetId="1" r:id="rId1"/>
@@ -59,8 +59,11 @@
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
-此处是1级的属性
-装备成长用公式做。</t>
+此处填升级固定值，等于是1级的属性
+装备成长用公式做。
+装备属性成长数值公式=(装备等级*各属性成长率+各属性固定值)*装备品质参数
+公式内取值分别对应配置表att、globalconfig
+</t>
         </r>
       </text>
     </comment>
@@ -69,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="108">
   <si>
     <t>行列头两行不会被读取</t>
   </si>
@@ -81,10 +84,8 @@
 对应att表id</t>
   </si>
   <si>
-    <t>0: 武器 -
-1: 衣服 -
+    <t>0: 武器
+1: 衣服
 2: 鞋子 
 3: 饰品</t>
   </si>
@@ -221,7 +222,7 @@
     <t>单手剑1</t>
   </si>
   <si>
-    <t>2001</t>
+    <t>2000</t>
   </si>
   <si>
     <t>单手剑2</t>
@@ -399,105 +400,6 @@
   </si>
   <si>
     <t>召唤物10</t>
-  </si>
-  <si>
-    <t>衣服1</t>
-  </si>
-  <si>
-    <t>2002</t>
-  </si>
-  <si>
-    <t>衣服2</t>
-  </si>
-  <si>
-    <t>衣服3</t>
-  </si>
-  <si>
-    <t>衣服4</t>
-  </si>
-  <si>
-    <t>衣服5</t>
-  </si>
-  <si>
-    <t>衣服6</t>
-  </si>
-  <si>
-    <t>衣服7</t>
-  </si>
-  <si>
-    <t>衣服8</t>
-  </si>
-  <si>
-    <t>衣服9</t>
-  </si>
-  <si>
-    <t>衣服10</t>
-  </si>
-  <si>
-    <t>裤子1</t>
-  </si>
-  <si>
-    <t>2003</t>
-  </si>
-  <si>
-    <t>裤子2</t>
-  </si>
-  <si>
-    <t>裤子3</t>
-  </si>
-  <si>
-    <t>裤子4</t>
-  </si>
-  <si>
-    <t>裤子5</t>
-  </si>
-  <si>
-    <t>裤子6</t>
-  </si>
-  <si>
-    <t>裤子7</t>
-  </si>
-  <si>
-    <t>裤子8</t>
-  </si>
-  <si>
-    <t>裤子9</t>
-  </si>
-  <si>
-    <t>裤子10</t>
-  </si>
-  <si>
-    <t>饰品1</t>
-  </si>
-  <si>
-    <t>2004</t>
-  </si>
-  <si>
-    <t>饰品2</t>
-  </si>
-  <si>
-    <t>饰品3</t>
-  </si>
-  <si>
-    <t>饰品4</t>
-  </si>
-  <si>
-    <t>饰品5</t>
-  </si>
-  <si>
-    <t>饰品6</t>
-  </si>
-  <si>
-    <t>饰品7</t>
-  </si>
-  <si>
-    <t>饰品8</t>
-  </si>
-  <si>
-    <t>饰品9</t>
-  </si>
-  <si>
-    <t>饰品10</t>
   </si>
 </sst>
 </file>
@@ -506,11 +408,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -531,21 +433,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
@@ -559,16 +454,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -582,11 +478,45 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Helvetica Neue"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -598,17 +528,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF0000FF"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -624,31 +546,25 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Helvetica Neue"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -659,26 +575,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <b/>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="36">
@@ -708,7 +621,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -720,13 +699,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -744,151 +801,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -917,11 +830,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -929,23 +848,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -961,17 +865,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -992,16 +885,25 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1014,151 +916,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1181,54 +1094,54 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="1" builtinId="52"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="2" builtinId="42"/>
-    <cellStyle name="强调文字颜色 4" xfId="3" builtinId="41"/>
-    <cellStyle name="输入" xfId="4" builtinId="20"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="5" builtinId="39"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="6" builtinId="38"/>
-    <cellStyle name="货币" xfId="7" builtinId="4"/>
-    <cellStyle name="强调文字颜色 3" xfId="8" builtinId="37"/>
-    <cellStyle name="百分比" xfId="9" builtinId="5"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="10" builtinId="36"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="11" builtinId="48"/>
-    <cellStyle name="强调文字颜色 2" xfId="12" builtinId="33"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="13" builtinId="32"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="14" builtinId="44"/>
-    <cellStyle name="计算" xfId="15" builtinId="22"/>
-    <cellStyle name="强调文字颜色 1" xfId="16" builtinId="29"/>
-    <cellStyle name="适中" xfId="17" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="18" builtinId="46"/>
-    <cellStyle name="好" xfId="19" builtinId="26"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="20" builtinId="30"/>
-    <cellStyle name="汇总" xfId="21" builtinId="25"/>
-    <cellStyle name="差" xfId="22" builtinId="27"/>
-    <cellStyle name="检查单元格" xfId="23" builtinId="23"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
     <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="标题 1" xfId="25" builtinId="16"/>
-    <cellStyle name="解释性文本" xfId="26" builtinId="53"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="27" builtinId="34"/>
-    <cellStyle name="标题 4" xfId="28" builtinId="19"/>
-    <cellStyle name="货币[0]" xfId="29" builtinId="7"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="30" builtinId="43"/>
-    <cellStyle name="千位分隔" xfId="31" builtinId="3"/>
-    <cellStyle name="已访问的超链接" xfId="32" builtinId="9"/>
-    <cellStyle name="标题" xfId="33" builtinId="15"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="34" builtinId="35"/>
-    <cellStyle name="警告文本" xfId="35" builtinId="11"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
-    <cellStyle name="注释" xfId="37" builtinId="10"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="38" builtinId="50"/>
-    <cellStyle name="强调文字颜色 5" xfId="39" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51"/>
-    <cellStyle name="超链接" xfId="41" builtinId="8"/>
-    <cellStyle name="千位分隔[0]" xfId="42" builtinId="6"/>
-    <cellStyle name="标题 2" xfId="43" builtinId="17"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
     <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="标题 3" xfId="45" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
     <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="47" builtinId="31"/>
-    <cellStyle name="链接单元格" xfId="48" builtinId="24"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0"/>
   <colors>
@@ -2376,34 +2289,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AA101"/>
+  <dimension ref="A1:AA71"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="AB18" sqref="AB18"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.25" defaultRowHeight="13.35" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="24.8461538461538" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.85" style="1" customWidth="1"/>
     <col min="2" max="2" width="19.25" style="1" customWidth="1"/>
     <col min="3" max="3" width="19.75" style="1" customWidth="1"/>
     <col min="4" max="4" width="19.25" style="1" customWidth="1"/>
     <col min="5" max="5" width="13.125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.53846153846154" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.4615384615385" style="1" customWidth="1"/>
-    <col min="8" max="12" width="12.9230769230769" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.54166666666667" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.4583333333333" style="1" customWidth="1"/>
+    <col min="8" max="12" width="12.925" style="1" customWidth="1"/>
     <col min="13" max="13" width="26.875" style="1" customWidth="1"/>
-    <col min="14" max="19" width="15.3846153846154" style="1" customWidth="1"/>
-    <col min="20" max="20" width="24.1538461538462" style="1" customWidth="1"/>
-    <col min="21" max="26" width="11.4615384615385" style="1" customWidth="1"/>
-    <col min="27" max="27" width="24.1538461538462" style="1" customWidth="1"/>
+    <col min="14" max="19" width="15.3833333333333" style="1" customWidth="1"/>
+    <col min="20" max="20" width="24.15" style="1" customWidth="1"/>
+    <col min="21" max="26" width="11.4583333333333" style="1" customWidth="1"/>
+    <col min="27" max="27" width="24.15" style="1" customWidth="1"/>
     <col min="28" max="16372" width="19.25" style="1" customWidth="1"/>
     <col min="16373" max="16384" width="19.25" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.8" spans="1:27">
+    <row r="1" ht="13.5" spans="1:27">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2434,7 +2347,7 @@
       <c r="Z1" s="3"/>
       <c r="AA1" s="3"/>
     </row>
-    <row r="2" ht="68" spans="1:27">
+    <row r="2" ht="54" spans="1:27">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="4" t="s">
@@ -7487,2420 +7400,20 @@
         <v>-1,1200,1201,1202,1203,1204</v>
       </c>
     </row>
-    <row r="67" customHeight="1" spans="3:27">
-      <c r="C67" s="6">
-        <v>1060</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E67" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="F67" s="6">
-        <v>1</v>
-      </c>
-      <c r="G67" s="6">
-        <v>2010</v>
-      </c>
-      <c r="H67" s="6">
-        <v>2010</v>
-      </c>
-      <c r="I67" s="6">
-        <v>2011</v>
-      </c>
-      <c r="J67" s="6">
-        <v>2012</v>
-      </c>
-      <c r="K67" s="6">
-        <v>2013</v>
-      </c>
-      <c r="L67" s="6">
-        <v>2014</v>
-      </c>
-      <c r="M67" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v>2010,2010,2011,2012,2013,2014</v>
-      </c>
-      <c r="N67" s="6">
-        <v>-1</v>
-      </c>
-      <c r="O67" s="6">
-        <v>1100011</v>
-      </c>
-      <c r="P67" s="6">
-        <v>1100012</v>
-      </c>
-      <c r="Q67" s="6">
-        <v>-1</v>
-      </c>
-      <c r="R67" s="6">
-        <v>-1</v>
-      </c>
-      <c r="S67" s="6">
-        <v>-1</v>
-      </c>
-      <c r="T67" s="6" t="str">
-        <f t="shared" si="4"/>
-        <v>-1,1100011,1100012,-1,-1,-1</v>
-      </c>
-      <c r="U67" s="6">
-        <v>-1</v>
-      </c>
-      <c r="V67" s="6">
-        <v>1200</v>
-      </c>
-      <c r="W67" s="6">
-        <v>1201</v>
-      </c>
-      <c r="X67" s="6">
-        <v>1202</v>
-      </c>
-      <c r="Y67" s="6">
-        <v>1203</v>
-      </c>
-      <c r="Z67" s="6">
-        <v>1204</v>
-      </c>
-      <c r="AA67" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v>-1,1200,1201,1202,1203,1204</v>
-      </c>
+    <row r="67" customHeight="1" spans="5:5">
+      <c r="E67" s="7"/>
     </row>
-    <row r="68" customHeight="1" spans="3:27">
-      <c r="C68" s="6">
-        <v>1061</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E68" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="F68" s="6">
-        <v>1</v>
-      </c>
-      <c r="G68" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H68" s="1">
-        <v>2020</v>
-      </c>
-      <c r="I68" s="1">
-        <v>2021</v>
-      </c>
-      <c r="J68" s="1">
-        <v>2022</v>
-      </c>
-      <c r="K68" s="1">
-        <v>2023</v>
-      </c>
-      <c r="L68" s="1">
-        <v>2024</v>
-      </c>
-      <c r="M68" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v>2020,2020,2021,2022,2023,2024</v>
-      </c>
-      <c r="N68" s="6">
-        <v>-1</v>
-      </c>
-      <c r="O68" s="6">
-        <v>1100011</v>
-      </c>
-      <c r="P68" s="6">
-        <v>1100012</v>
-      </c>
-      <c r="Q68" s="6">
-        <v>-1</v>
-      </c>
-      <c r="R68" s="6">
-        <v>-1</v>
-      </c>
-      <c r="S68" s="6">
-        <v>-1</v>
-      </c>
-      <c r="T68" s="6" t="str">
-        <f t="shared" si="4"/>
-        <v>-1,1100011,1100012,-1,-1,-1</v>
-      </c>
-      <c r="U68" s="6">
-        <v>-1</v>
-      </c>
-      <c r="V68" s="6">
-        <v>1200</v>
-      </c>
-      <c r="W68" s="6">
-        <v>1201</v>
-      </c>
-      <c r="X68" s="6">
-        <v>1202</v>
-      </c>
-      <c r="Y68" s="6">
-        <v>1203</v>
-      </c>
-      <c r="Z68" s="6">
-        <v>1204</v>
-      </c>
-      <c r="AA68" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v>-1,1200,1201,1202,1203,1204</v>
-      </c>
+    <row r="68" customHeight="1" spans="5:5">
+      <c r="E68" s="7"/>
     </row>
-    <row r="69" customHeight="1" spans="3:27">
-      <c r="C69" s="6">
-        <v>1062</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E69" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="F69" s="6">
-        <v>1</v>
-      </c>
-      <c r="G69" s="6">
-        <v>2010</v>
-      </c>
-      <c r="H69" s="6">
-        <v>2010</v>
-      </c>
-      <c r="I69" s="6">
-        <v>2011</v>
-      </c>
-      <c r="J69" s="6">
-        <v>2012</v>
-      </c>
-      <c r="K69" s="6">
-        <v>2013</v>
-      </c>
-      <c r="L69" s="6">
-        <v>2014</v>
-      </c>
-      <c r="M69" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v>2010,2010,2011,2012,2013,2014</v>
-      </c>
-      <c r="N69" s="6">
-        <v>-1</v>
-      </c>
-      <c r="O69" s="6">
-        <v>1100011</v>
-      </c>
-      <c r="P69" s="6">
-        <v>1100012</v>
-      </c>
-      <c r="Q69" s="6">
-        <v>-1</v>
-      </c>
-      <c r="R69" s="6">
-        <v>-1</v>
-      </c>
-      <c r="S69" s="6">
-        <v>-1</v>
-      </c>
-      <c r="T69" s="6" t="str">
-        <f t="shared" si="4"/>
-        <v>-1,1100011,1100012,-1,-1,-1</v>
-      </c>
-      <c r="U69" s="6">
-        <v>-1</v>
-      </c>
-      <c r="V69" s="6">
-        <v>1200</v>
-      </c>
-      <c r="W69" s="6">
-        <v>1201</v>
-      </c>
-      <c r="X69" s="6">
-        <v>1202</v>
-      </c>
-      <c r="Y69" s="6">
-        <v>1203</v>
-      </c>
-      <c r="Z69" s="6">
-        <v>1204</v>
-      </c>
-      <c r="AA69" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v>-1,1200,1201,1202,1203,1204</v>
-      </c>
+    <row r="69" customHeight="1" spans="5:5">
+      <c r="E69" s="7"/>
     </row>
-    <row r="70" customHeight="1" spans="3:27">
-      <c r="C70" s="6">
-        <v>1063</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E70" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="F70" s="6">
-        <v>1</v>
-      </c>
-      <c r="G70" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H70" s="1">
-        <v>2020</v>
-      </c>
-      <c r="I70" s="1">
-        <v>2021</v>
-      </c>
-      <c r="J70" s="1">
-        <v>2022</v>
-      </c>
-      <c r="K70" s="1">
-        <v>2023</v>
-      </c>
-      <c r="L70" s="1">
-        <v>2024</v>
-      </c>
-      <c r="M70" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v>2020,2020,2021,2022,2023,2024</v>
-      </c>
-      <c r="N70" s="6">
-        <v>-1</v>
-      </c>
-      <c r="O70" s="6">
-        <v>1100011</v>
-      </c>
-      <c r="P70" s="6">
-        <v>1100012</v>
-      </c>
-      <c r="Q70" s="6">
-        <v>-1</v>
-      </c>
-      <c r="R70" s="6">
-        <v>-1</v>
-      </c>
-      <c r="S70" s="6">
-        <v>-1</v>
-      </c>
-      <c r="T70" s="6" t="str">
-        <f t="shared" si="4"/>
-        <v>-1,1100011,1100012,-1,-1,-1</v>
-      </c>
-      <c r="U70" s="6">
-        <v>-1</v>
-      </c>
-      <c r="V70" s="6">
-        <v>1200</v>
-      </c>
-      <c r="W70" s="6">
-        <v>1201</v>
-      </c>
-      <c r="X70" s="6">
-        <v>1202</v>
-      </c>
-      <c r="Y70" s="6">
-        <v>1203</v>
-      </c>
-      <c r="Z70" s="6">
-        <v>1204</v>
-      </c>
-      <c r="AA70" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v>-1,1200,1201,1202,1203,1204</v>
-      </c>
+    <row r="70" customHeight="1" spans="5:5">
+      <c r="E70" s="7"/>
     </row>
-    <row r="71" customHeight="1" spans="3:27">
-      <c r="C71" s="6">
-        <v>1064</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E71" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="F71" s="6">
-        <v>1</v>
-      </c>
-      <c r="G71" s="6">
-        <v>2010</v>
-      </c>
-      <c r="H71" s="6">
-        <v>2010</v>
-      </c>
-      <c r="I71" s="6">
-        <v>2011</v>
-      </c>
-      <c r="J71" s="6">
-        <v>2012</v>
-      </c>
-      <c r="K71" s="6">
-        <v>2013</v>
-      </c>
-      <c r="L71" s="6">
-        <v>2014</v>
-      </c>
-      <c r="M71" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v>2010,2010,2011,2012,2013,2014</v>
-      </c>
-      <c r="N71" s="6">
-        <v>-1</v>
-      </c>
-      <c r="O71" s="6">
-        <v>1100011</v>
-      </c>
-      <c r="P71" s="6">
-        <v>1100012</v>
-      </c>
-      <c r="Q71" s="6">
-        <v>-1</v>
-      </c>
-      <c r="R71" s="6">
-        <v>-1</v>
-      </c>
-      <c r="S71" s="6">
-        <v>-1</v>
-      </c>
-      <c r="T71" s="6" t="str">
-        <f t="shared" si="4"/>
-        <v>-1,1100011,1100012,-1,-1,-1</v>
-      </c>
-      <c r="U71" s="6">
-        <v>-1</v>
-      </c>
-      <c r="V71" s="6">
-        <v>1200</v>
-      </c>
-      <c r="W71" s="6">
-        <v>1201</v>
-      </c>
-      <c r="X71" s="6">
-        <v>1202</v>
-      </c>
-      <c r="Y71" s="6">
-        <v>1203</v>
-      </c>
-      <c r="Z71" s="6">
-        <v>1204</v>
-      </c>
-      <c r="AA71" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v>-1,1200,1201,1202,1203,1204</v>
-      </c>
-    </row>
-    <row r="72" customHeight="1" spans="3:27">
-      <c r="C72" s="6">
-        <v>1065</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E72" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="F72" s="6">
-        <v>1</v>
-      </c>
-      <c r="G72" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H72" s="1">
-        <v>2020</v>
-      </c>
-      <c r="I72" s="1">
-        <v>2021</v>
-      </c>
-      <c r="J72" s="1">
-        <v>2022</v>
-      </c>
-      <c r="K72" s="1">
-        <v>2023</v>
-      </c>
-      <c r="L72" s="1">
-        <v>2024</v>
-      </c>
-      <c r="M72" s="6" t="str">
-        <f t="shared" ref="M72:M96" si="6">G72&amp;","&amp;H72&amp;","&amp;I72&amp;","&amp;J72&amp;","&amp;K72&amp;","&amp;L72</f>
-        <v>2020,2020,2021,2022,2023,2024</v>
-      </c>
-      <c r="N72" s="6">
-        <v>-1</v>
-      </c>
-      <c r="O72" s="6">
-        <v>1100011</v>
-      </c>
-      <c r="P72" s="6">
-        <v>1100012</v>
-      </c>
-      <c r="Q72" s="6">
-        <v>-1</v>
-      </c>
-      <c r="R72" s="6">
-        <v>-1</v>
-      </c>
-      <c r="S72" s="6">
-        <v>-1</v>
-      </c>
-      <c r="T72" s="6" t="str">
-        <f t="shared" ref="T72:T96" si="7">N72&amp;","&amp;O72&amp;","&amp;P72&amp;","&amp;Q72&amp;","&amp;R72&amp;","&amp;S72</f>
-        <v>-1,1100011,1100012,-1,-1,-1</v>
-      </c>
-      <c r="U72" s="6">
-        <v>-1</v>
-      </c>
-      <c r="V72" s="6">
-        <v>1200</v>
-      </c>
-      <c r="W72" s="6">
-        <v>1201</v>
-      </c>
-      <c r="X72" s="6">
-        <v>1202</v>
-      </c>
-      <c r="Y72" s="6">
-        <v>1203</v>
-      </c>
-      <c r="Z72" s="6">
-        <v>1204</v>
-      </c>
-      <c r="AA72" s="6" t="str">
-        <f t="shared" ref="AA72:AA96" si="8">U72&amp;","&amp;V72&amp;","&amp;W72&amp;","&amp;X72&amp;","&amp;Y72&amp;","&amp;Z72</f>
-        <v>-1,1200,1201,1202,1203,1204</v>
-      </c>
-    </row>
-    <row r="73" customHeight="1" spans="3:27">
-      <c r="C73" s="6">
-        <v>1066</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E73" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="F73" s="6">
-        <v>1</v>
-      </c>
-      <c r="G73" s="6">
-        <v>2010</v>
-      </c>
-      <c r="H73" s="6">
-        <v>2010</v>
-      </c>
-      <c r="I73" s="6">
-        <v>2011</v>
-      </c>
-      <c r="J73" s="6">
-        <v>2012</v>
-      </c>
-      <c r="K73" s="6">
-        <v>2013</v>
-      </c>
-      <c r="L73" s="6">
-        <v>2014</v>
-      </c>
-      <c r="M73" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>2010,2010,2011,2012,2013,2014</v>
-      </c>
-      <c r="N73" s="6">
-        <v>-1</v>
-      </c>
-      <c r="O73" s="6">
-        <v>1100011</v>
-      </c>
-      <c r="P73" s="6">
-        <v>1100012</v>
-      </c>
-      <c r="Q73" s="6">
-        <v>-1</v>
-      </c>
-      <c r="R73" s="6">
-        <v>-1</v>
-      </c>
-      <c r="S73" s="6">
-        <v>-1</v>
-      </c>
-      <c r="T73" s="6" t="str">
-        <f t="shared" si="7"/>
-        <v>-1,1100011,1100012,-1,-1,-1</v>
-      </c>
-      <c r="U73" s="6">
-        <v>-1</v>
-      </c>
-      <c r="V73" s="6">
-        <v>1200</v>
-      </c>
-      <c r="W73" s="6">
-        <v>1201</v>
-      </c>
-      <c r="X73" s="6">
-        <v>1202</v>
-      </c>
-      <c r="Y73" s="6">
-        <v>1203</v>
-      </c>
-      <c r="Z73" s="6">
-        <v>1204</v>
-      </c>
-      <c r="AA73" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v>-1,1200,1201,1202,1203,1204</v>
-      </c>
-    </row>
-    <row r="74" customHeight="1" spans="3:27">
-      <c r="C74" s="6">
-        <v>1067</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E74" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="F74" s="6">
-        <v>1</v>
-      </c>
-      <c r="G74" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H74" s="1">
-        <v>2020</v>
-      </c>
-      <c r="I74" s="1">
-        <v>2021</v>
-      </c>
-      <c r="J74" s="1">
-        <v>2022</v>
-      </c>
-      <c r="K74" s="1">
-        <v>2023</v>
-      </c>
-      <c r="L74" s="1">
-        <v>2024</v>
-      </c>
-      <c r="M74" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>2020,2020,2021,2022,2023,2024</v>
-      </c>
-      <c r="N74" s="6">
-        <v>-1</v>
-      </c>
-      <c r="O74" s="6">
-        <v>1100011</v>
-      </c>
-      <c r="P74" s="6">
-        <v>1100012</v>
-      </c>
-      <c r="Q74" s="6">
-        <v>-1</v>
-      </c>
-      <c r="R74" s="6">
-        <v>-1</v>
-      </c>
-      <c r="S74" s="6">
-        <v>-1</v>
-      </c>
-      <c r="T74" s="6" t="str">
-        <f t="shared" si="7"/>
-        <v>-1,1100011,1100012,-1,-1,-1</v>
-      </c>
-      <c r="U74" s="6">
-        <v>-1</v>
-      </c>
-      <c r="V74" s="6">
-        <v>1200</v>
-      </c>
-      <c r="W74" s="6">
-        <v>1201</v>
-      </c>
-      <c r="X74" s="6">
-        <v>1202</v>
-      </c>
-      <c r="Y74" s="6">
-        <v>1203</v>
-      </c>
-      <c r="Z74" s="6">
-        <v>1204</v>
-      </c>
-      <c r="AA74" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v>-1,1200,1201,1202,1203,1204</v>
-      </c>
-    </row>
-    <row r="75" customHeight="1" spans="3:27">
-      <c r="C75" s="6">
-        <v>1068</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E75" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="F75" s="6">
-        <v>1</v>
-      </c>
-      <c r="G75" s="6">
-        <v>2010</v>
-      </c>
-      <c r="H75" s="6">
-        <v>2010</v>
-      </c>
-      <c r="I75" s="6">
-        <v>2011</v>
-      </c>
-      <c r="J75" s="6">
-        <v>2012</v>
-      </c>
-      <c r="K75" s="6">
-        <v>2013</v>
-      </c>
-      <c r="L75" s="6">
-        <v>2014</v>
-      </c>
-      <c r="M75" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>2010,2010,2011,2012,2013,2014</v>
-      </c>
-      <c r="N75" s="6">
-        <v>-1</v>
-      </c>
-      <c r="O75" s="6">
-        <v>1100011</v>
-      </c>
-      <c r="P75" s="6">
-        <v>1100012</v>
-      </c>
-      <c r="Q75" s="6">
-        <v>-1</v>
-      </c>
-      <c r="R75" s="6">
-        <v>-1</v>
-      </c>
-      <c r="S75" s="6">
-        <v>-1</v>
-      </c>
-      <c r="T75" s="6" t="str">
-        <f t="shared" si="7"/>
-        <v>-1,1100011,1100012,-1,-1,-1</v>
-      </c>
-      <c r="U75" s="6">
-        <v>-1</v>
-      </c>
-      <c r="V75" s="6">
-        <v>1200</v>
-      </c>
-      <c r="W75" s="6">
-        <v>1201</v>
-      </c>
-      <c r="X75" s="6">
-        <v>1202</v>
-      </c>
-      <c r="Y75" s="6">
-        <v>1203</v>
-      </c>
-      <c r="Z75" s="6">
-        <v>1204</v>
-      </c>
-      <c r="AA75" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v>-1,1200,1201,1202,1203,1204</v>
-      </c>
-    </row>
-    <row r="76" customHeight="1" spans="3:27">
-      <c r="C76" s="6">
-        <v>1069</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E76" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="F76" s="6">
-        <v>1</v>
-      </c>
-      <c r="G76" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H76" s="1">
-        <v>2020</v>
-      </c>
-      <c r="I76" s="1">
-        <v>2021</v>
-      </c>
-      <c r="J76" s="1">
-        <v>2022</v>
-      </c>
-      <c r="K76" s="1">
-        <v>2023</v>
-      </c>
-      <c r="L76" s="1">
-        <v>2024</v>
-      </c>
-      <c r="M76" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>2020,2020,2021,2022,2023,2024</v>
-      </c>
-      <c r="N76" s="6">
-        <v>-1</v>
-      </c>
-      <c r="O76" s="6">
-        <v>1100011</v>
-      </c>
-      <c r="P76" s="6">
-        <v>1100012</v>
-      </c>
-      <c r="Q76" s="6">
-        <v>-1</v>
-      </c>
-      <c r="R76" s="6">
-        <v>-1</v>
-      </c>
-      <c r="S76" s="6">
-        <v>-1</v>
-      </c>
-      <c r="T76" s="6" t="str">
-        <f t="shared" si="7"/>
-        <v>-1,1100011,1100012,-1,-1,-1</v>
-      </c>
-      <c r="U76" s="6">
-        <v>-1</v>
-      </c>
-      <c r="V76" s="6">
-        <v>1200</v>
-      </c>
-      <c r="W76" s="6">
-        <v>1201</v>
-      </c>
-      <c r="X76" s="6">
-        <v>1202</v>
-      </c>
-      <c r="Y76" s="6">
-        <v>1203</v>
-      </c>
-      <c r="Z76" s="6">
-        <v>1204</v>
-      </c>
-      <c r="AA76" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v>-1,1200,1201,1202,1203,1204</v>
-      </c>
-    </row>
-    <row r="77" customHeight="1" spans="3:27">
-      <c r="C77" s="6">
-        <v>1070</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E77" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="F77" s="1">
-        <v>2</v>
-      </c>
-      <c r="G77" s="6">
-        <v>2010</v>
-      </c>
-      <c r="H77" s="6">
-        <v>2010</v>
-      </c>
-      <c r="I77" s="6">
-        <v>2011</v>
-      </c>
-      <c r="J77" s="6">
-        <v>2012</v>
-      </c>
-      <c r="K77" s="6">
-        <v>2013</v>
-      </c>
-      <c r="L77" s="6">
-        <v>2014</v>
-      </c>
-      <c r="M77" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>2010,2010,2011,2012,2013,2014</v>
-      </c>
-      <c r="N77" s="6">
-        <v>-1</v>
-      </c>
-      <c r="O77" s="6">
-        <v>1100011</v>
-      </c>
-      <c r="P77" s="6">
-        <v>1100012</v>
-      </c>
-      <c r="Q77" s="6">
-        <v>-1</v>
-      </c>
-      <c r="R77" s="6">
-        <v>-1</v>
-      </c>
-      <c r="S77" s="6">
-        <v>-1</v>
-      </c>
-      <c r="T77" s="6" t="str">
-        <f t="shared" si="7"/>
-        <v>-1,1100011,1100012,-1,-1,-1</v>
-      </c>
-      <c r="U77" s="6">
-        <v>-1</v>
-      </c>
-      <c r="V77" s="6">
-        <v>1200</v>
-      </c>
-      <c r="W77" s="6">
-        <v>1201</v>
-      </c>
-      <c r="X77" s="6">
-        <v>1202</v>
-      </c>
-      <c r="Y77" s="6">
-        <v>1203</v>
-      </c>
-      <c r="Z77" s="6">
-        <v>1204</v>
-      </c>
-      <c r="AA77" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v>-1,1200,1201,1202,1203,1204</v>
-      </c>
-    </row>
-    <row r="78" customHeight="1" spans="3:27">
-      <c r="C78" s="6">
-        <v>1071</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E78" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="F78" s="1">
-        <v>2</v>
-      </c>
-      <c r="G78" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H78" s="1">
-        <v>2020</v>
-      </c>
-      <c r="I78" s="1">
-        <v>2021</v>
-      </c>
-      <c r="J78" s="1">
-        <v>2022</v>
-      </c>
-      <c r="K78" s="1">
-        <v>2023</v>
-      </c>
-      <c r="L78" s="1">
-        <v>2024</v>
-      </c>
-      <c r="M78" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>2020,2020,2021,2022,2023,2024</v>
-      </c>
-      <c r="N78" s="6">
-        <v>-1</v>
-      </c>
-      <c r="O78" s="6">
-        <v>1100011</v>
-      </c>
-      <c r="P78" s="6">
-        <v>1100012</v>
-      </c>
-      <c r="Q78" s="6">
-        <v>-1</v>
-      </c>
-      <c r="R78" s="6">
-        <v>-1</v>
-      </c>
-      <c r="S78" s="6">
-        <v>-1</v>
-      </c>
-      <c r="T78" s="6" t="str">
-        <f t="shared" si="7"/>
-        <v>-1,1100011,1100012,-1,-1,-1</v>
-      </c>
-      <c r="U78" s="6">
-        <v>-1</v>
-      </c>
-      <c r="V78" s="6">
-        <v>1200</v>
-      </c>
-      <c r="W78" s="6">
-        <v>1201</v>
-      </c>
-      <c r="X78" s="6">
-        <v>1202</v>
-      </c>
-      <c r="Y78" s="6">
-        <v>1203</v>
-      </c>
-      <c r="Z78" s="6">
-        <v>1204</v>
-      </c>
-      <c r="AA78" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v>-1,1200,1201,1202,1203,1204</v>
-      </c>
-    </row>
-    <row r="79" customHeight="1" spans="3:27">
-      <c r="C79" s="6">
-        <v>1072</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E79" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="F79" s="1">
-        <v>2</v>
-      </c>
-      <c r="G79" s="6">
-        <v>2010</v>
-      </c>
-      <c r="H79" s="6">
-        <v>2010</v>
-      </c>
-      <c r="I79" s="6">
-        <v>2011</v>
-      </c>
-      <c r="J79" s="6">
-        <v>2012</v>
-      </c>
-      <c r="K79" s="6">
-        <v>2013</v>
-      </c>
-      <c r="L79" s="6">
-        <v>2014</v>
-      </c>
-      <c r="M79" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>2010,2010,2011,2012,2013,2014</v>
-      </c>
-      <c r="N79" s="6">
-        <v>-1</v>
-      </c>
-      <c r="O79" s="6">
-        <v>1100011</v>
-      </c>
-      <c r="P79" s="6">
-        <v>1100012</v>
-      </c>
-      <c r="Q79" s="6">
-        <v>-1</v>
-      </c>
-      <c r="R79" s="6">
-        <v>-1</v>
-      </c>
-      <c r="S79" s="6">
-        <v>-1</v>
-      </c>
-      <c r="T79" s="6" t="str">
-        <f t="shared" si="7"/>
-        <v>-1,1100011,1100012,-1,-1,-1</v>
-      </c>
-      <c r="U79" s="6">
-        <v>-1</v>
-      </c>
-      <c r="V79" s="6">
-        <v>1200</v>
-      </c>
-      <c r="W79" s="6">
-        <v>1201</v>
-      </c>
-      <c r="X79" s="6">
-        <v>1202</v>
-      </c>
-      <c r="Y79" s="6">
-        <v>1203</v>
-      </c>
-      <c r="Z79" s="6">
-        <v>1204</v>
-      </c>
-      <c r="AA79" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v>-1,1200,1201,1202,1203,1204</v>
-      </c>
-    </row>
-    <row r="80" customHeight="1" spans="3:27">
-      <c r="C80" s="6">
-        <v>1073</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E80" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="F80" s="1">
-        <v>2</v>
-      </c>
-      <c r="G80" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H80" s="1">
-        <v>2020</v>
-      </c>
-      <c r="I80" s="1">
-        <v>2021</v>
-      </c>
-      <c r="J80" s="1">
-        <v>2022</v>
-      </c>
-      <c r="K80" s="1">
-        <v>2023</v>
-      </c>
-      <c r="L80" s="1">
-        <v>2024</v>
-      </c>
-      <c r="M80" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>2020,2020,2021,2022,2023,2024</v>
-      </c>
-      <c r="N80" s="6">
-        <v>-1</v>
-      </c>
-      <c r="O80" s="6">
-        <v>1100011</v>
-      </c>
-      <c r="P80" s="6">
-        <v>1100012</v>
-      </c>
-      <c r="Q80" s="6">
-        <v>-1</v>
-      </c>
-      <c r="R80" s="6">
-        <v>-1</v>
-      </c>
-      <c r="S80" s="6">
-        <v>-1</v>
-      </c>
-      <c r="T80" s="6" t="str">
-        <f t="shared" si="7"/>
-        <v>-1,1100011,1100012,-1,-1,-1</v>
-      </c>
-      <c r="U80" s="6">
-        <v>-1</v>
-      </c>
-      <c r="V80" s="6">
-        <v>1200</v>
-      </c>
-      <c r="W80" s="6">
-        <v>1201</v>
-      </c>
-      <c r="X80" s="6">
-        <v>1202</v>
-      </c>
-      <c r="Y80" s="6">
-        <v>1203</v>
-      </c>
-      <c r="Z80" s="6">
-        <v>1204</v>
-      </c>
-      <c r="AA80" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v>-1,1200,1201,1202,1203,1204</v>
-      </c>
-    </row>
-    <row r="81" customHeight="1" spans="3:27">
-      <c r="C81" s="6">
-        <v>1074</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="E81" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="F81" s="1">
-        <v>2</v>
-      </c>
-      <c r="G81" s="6">
-        <v>2010</v>
-      </c>
-      <c r="H81" s="6">
-        <v>2010</v>
-      </c>
-      <c r="I81" s="6">
-        <v>2011</v>
-      </c>
-      <c r="J81" s="6">
-        <v>2012</v>
-      </c>
-      <c r="K81" s="6">
-        <v>2013</v>
-      </c>
-      <c r="L81" s="6">
-        <v>2014</v>
-      </c>
-      <c r="M81" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>2010,2010,2011,2012,2013,2014</v>
-      </c>
-      <c r="N81" s="6">
-        <v>-1</v>
-      </c>
-      <c r="O81" s="6">
-        <v>1100011</v>
-      </c>
-      <c r="P81" s="6">
-        <v>1100012</v>
-      </c>
-      <c r="Q81" s="6">
-        <v>-1</v>
-      </c>
-      <c r="R81" s="6">
-        <v>-1</v>
-      </c>
-      <c r="S81" s="6">
-        <v>-1</v>
-      </c>
-      <c r="T81" s="6" t="str">
-        <f t="shared" si="7"/>
-        <v>-1,1100011,1100012,-1,-1,-1</v>
-      </c>
-      <c r="U81" s="6">
-        <v>-1</v>
-      </c>
-      <c r="V81" s="6">
-        <v>1200</v>
-      </c>
-      <c r="W81" s="6">
-        <v>1201</v>
-      </c>
-      <c r="X81" s="6">
-        <v>1202</v>
-      </c>
-      <c r="Y81" s="6">
-        <v>1203</v>
-      </c>
-      <c r="Z81" s="6">
-        <v>1204</v>
-      </c>
-      <c r="AA81" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v>-1,1200,1201,1202,1203,1204</v>
-      </c>
-    </row>
-    <row r="82" customHeight="1" spans="3:27">
-      <c r="C82" s="6">
-        <v>1075</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E82" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="F82" s="1">
-        <v>2</v>
-      </c>
-      <c r="G82" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H82" s="1">
-        <v>2020</v>
-      </c>
-      <c r="I82" s="1">
-        <v>2021</v>
-      </c>
-      <c r="J82" s="1">
-        <v>2022</v>
-      </c>
-      <c r="K82" s="1">
-        <v>2023</v>
-      </c>
-      <c r="L82" s="1">
-        <v>2024</v>
-      </c>
-      <c r="M82" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>2020,2020,2021,2022,2023,2024</v>
-      </c>
-      <c r="N82" s="6">
-        <v>-1</v>
-      </c>
-      <c r="O82" s="6">
-        <v>1100011</v>
-      </c>
-      <c r="P82" s="6">
-        <v>1100012</v>
-      </c>
-      <c r="Q82" s="6">
-        <v>-1</v>
-      </c>
-      <c r="R82" s="6">
-        <v>-1</v>
-      </c>
-      <c r="S82" s="6">
-        <v>-1</v>
-      </c>
-      <c r="T82" s="6" t="str">
-        <f t="shared" si="7"/>
-        <v>-1,1100011,1100012,-1,-1,-1</v>
-      </c>
-      <c r="U82" s="6">
-        <v>-1</v>
-      </c>
-      <c r="V82" s="6">
-        <v>1200</v>
-      </c>
-      <c r="W82" s="6">
-        <v>1201</v>
-      </c>
-      <c r="X82" s="6">
-        <v>1202</v>
-      </c>
-      <c r="Y82" s="6">
-        <v>1203</v>
-      </c>
-      <c r="Z82" s="6">
-        <v>1204</v>
-      </c>
-      <c r="AA82" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v>-1,1200,1201,1202,1203,1204</v>
-      </c>
-    </row>
-    <row r="83" customHeight="1" spans="3:27">
-      <c r="C83" s="6">
-        <v>1076</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E83" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="F83" s="1">
-        <v>2</v>
-      </c>
-      <c r="G83" s="6">
-        <v>2010</v>
-      </c>
-      <c r="H83" s="6">
-        <v>2010</v>
-      </c>
-      <c r="I83" s="6">
-        <v>2011</v>
-      </c>
-      <c r="J83" s="6">
-        <v>2012</v>
-      </c>
-      <c r="K83" s="6">
-        <v>2013</v>
-      </c>
-      <c r="L83" s="6">
-        <v>2014</v>
-      </c>
-      <c r="M83" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>2010,2010,2011,2012,2013,2014</v>
-      </c>
-      <c r="N83" s="6">
-        <v>-1</v>
-      </c>
-      <c r="O83" s="6">
-        <v>1100011</v>
-      </c>
-      <c r="P83" s="6">
-        <v>1100012</v>
-      </c>
-      <c r="Q83" s="6">
-        <v>-1</v>
-      </c>
-      <c r="R83" s="6">
-        <v>-1</v>
-      </c>
-      <c r="S83" s="6">
-        <v>-1</v>
-      </c>
-      <c r="T83" s="6" t="str">
-        <f t="shared" si="7"/>
-        <v>-1,1100011,1100012,-1,-1,-1</v>
-      </c>
-      <c r="U83" s="6">
-        <v>-1</v>
-      </c>
-      <c r="V83" s="6">
-        <v>1200</v>
-      </c>
-      <c r="W83" s="6">
-        <v>1201</v>
-      </c>
-      <c r="X83" s="6">
-        <v>1202</v>
-      </c>
-      <c r="Y83" s="6">
-        <v>1203</v>
-      </c>
-      <c r="Z83" s="6">
-        <v>1204</v>
-      </c>
-      <c r="AA83" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v>-1,1200,1201,1202,1203,1204</v>
-      </c>
-    </row>
-    <row r="84" customHeight="1" spans="3:27">
-      <c r="C84" s="6">
-        <v>1077</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E84" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="F84" s="1">
-        <v>2</v>
-      </c>
-      <c r="G84" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H84" s="1">
-        <v>2020</v>
-      </c>
-      <c r="I84" s="1">
-        <v>2021</v>
-      </c>
-      <c r="J84" s="1">
-        <v>2022</v>
-      </c>
-      <c r="K84" s="1">
-        <v>2023</v>
-      </c>
-      <c r="L84" s="1">
-        <v>2024</v>
-      </c>
-      <c r="M84" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>2020,2020,2021,2022,2023,2024</v>
-      </c>
-      <c r="N84" s="6">
-        <v>-1</v>
-      </c>
-      <c r="O84" s="6">
-        <v>1100011</v>
-      </c>
-      <c r="P84" s="6">
-        <v>1100012</v>
-      </c>
-      <c r="Q84" s="6">
-        <v>-1</v>
-      </c>
-      <c r="R84" s="6">
-        <v>-1</v>
-      </c>
-      <c r="S84" s="6">
-        <v>-1</v>
-      </c>
-      <c r="T84" s="6" t="str">
-        <f t="shared" si="7"/>
-        <v>-1,1100011,1100012,-1,-1,-1</v>
-      </c>
-      <c r="U84" s="6">
-        <v>-1</v>
-      </c>
-      <c r="V84" s="6">
-        <v>1200</v>
-      </c>
-      <c r="W84" s="6">
-        <v>1201</v>
-      </c>
-      <c r="X84" s="6">
-        <v>1202</v>
-      </c>
-      <c r="Y84" s="6">
-        <v>1203</v>
-      </c>
-      <c r="Z84" s="6">
-        <v>1204</v>
-      </c>
-      <c r="AA84" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v>-1,1200,1201,1202,1203,1204</v>
-      </c>
-    </row>
-    <row r="85" customHeight="1" spans="3:27">
-      <c r="C85" s="6">
-        <v>1078</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E85" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="F85" s="1">
-        <v>2</v>
-      </c>
-      <c r="G85" s="6">
-        <v>2010</v>
-      </c>
-      <c r="H85" s="6">
-        <v>2010</v>
-      </c>
-      <c r="I85" s="6">
-        <v>2011</v>
-      </c>
-      <c r="J85" s="6">
-        <v>2012</v>
-      </c>
-      <c r="K85" s="6">
-        <v>2013</v>
-      </c>
-      <c r="L85" s="6">
-        <v>2014</v>
-      </c>
-      <c r="M85" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>2010,2010,2011,2012,2013,2014</v>
-      </c>
-      <c r="N85" s="6">
-        <v>-1</v>
-      </c>
-      <c r="O85" s="6">
-        <v>1100011</v>
-      </c>
-      <c r="P85" s="6">
-        <v>1100012</v>
-      </c>
-      <c r="Q85" s="6">
-        <v>-1</v>
-      </c>
-      <c r="R85" s="6">
-        <v>-1</v>
-      </c>
-      <c r="S85" s="6">
-        <v>-1</v>
-      </c>
-      <c r="T85" s="6" t="str">
-        <f t="shared" si="7"/>
-        <v>-1,1100011,1100012,-1,-1,-1</v>
-      </c>
-      <c r="U85" s="6">
-        <v>-1</v>
-      </c>
-      <c r="V85" s="6">
-        <v>1200</v>
-      </c>
-      <c r="W85" s="6">
-        <v>1201</v>
-      </c>
-      <c r="X85" s="6">
-        <v>1202</v>
-      </c>
-      <c r="Y85" s="6">
-        <v>1203</v>
-      </c>
-      <c r="Z85" s="6">
-        <v>1204</v>
-      </c>
-      <c r="AA85" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v>-1,1200,1201,1202,1203,1204</v>
-      </c>
-    </row>
-    <row r="86" customHeight="1" spans="3:27">
-      <c r="C86" s="6">
-        <v>1079</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E86" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="F86" s="1">
-        <v>2</v>
-      </c>
-      <c r="G86" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H86" s="1">
-        <v>2020</v>
-      </c>
-      <c r="I86" s="1">
-        <v>2021</v>
-      </c>
-      <c r="J86" s="1">
-        <v>2022</v>
-      </c>
-      <c r="K86" s="1">
-        <v>2023</v>
-      </c>
-      <c r="L86" s="1">
-        <v>2024</v>
-      </c>
-      <c r="M86" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>2020,2020,2021,2022,2023,2024</v>
-      </c>
-      <c r="N86" s="6">
-        <v>-1</v>
-      </c>
-      <c r="O86" s="6">
-        <v>1100011</v>
-      </c>
-      <c r="P86" s="6">
-        <v>1100012</v>
-      </c>
-      <c r="Q86" s="6">
-        <v>-1</v>
-      </c>
-      <c r="R86" s="6">
-        <v>-1</v>
-      </c>
-      <c r="S86" s="6">
-        <v>-1</v>
-      </c>
-      <c r="T86" s="6" t="str">
-        <f t="shared" si="7"/>
-        <v>-1,1100011,1100012,-1,-1,-1</v>
-      </c>
-      <c r="U86" s="6">
-        <v>-1</v>
-      </c>
-      <c r="V86" s="6">
-        <v>1200</v>
-      </c>
-      <c r="W86" s="6">
-        <v>1201</v>
-      </c>
-      <c r="X86" s="6">
-        <v>1202</v>
-      </c>
-      <c r="Y86" s="6">
-        <v>1203</v>
-      </c>
-      <c r="Z86" s="6">
-        <v>1204</v>
-      </c>
-      <c r="AA86" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v>-1,1200,1201,1202,1203,1204</v>
-      </c>
-    </row>
-    <row r="87" customHeight="1" spans="3:27">
-      <c r="C87" s="6">
-        <v>1080</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E87" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="F87" s="1">
-        <v>3</v>
-      </c>
-      <c r="G87" s="6">
-        <v>2010</v>
-      </c>
-      <c r="H87" s="6">
-        <v>2010</v>
-      </c>
-      <c r="I87" s="6">
-        <v>2011</v>
-      </c>
-      <c r="J87" s="6">
-        <v>2012</v>
-      </c>
-      <c r="K87" s="6">
-        <v>2013</v>
-      </c>
-      <c r="L87" s="6">
-        <v>2014</v>
-      </c>
-      <c r="M87" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>2010,2010,2011,2012,2013,2014</v>
-      </c>
-      <c r="N87" s="6">
-        <v>-1</v>
-      </c>
-      <c r="O87" s="6">
-        <v>1100011</v>
-      </c>
-      <c r="P87" s="6">
-        <v>1100012</v>
-      </c>
-      <c r="Q87" s="6">
-        <v>-1</v>
-      </c>
-      <c r="R87" s="6">
-        <v>-1</v>
-      </c>
-      <c r="S87" s="6">
-        <v>-1</v>
-      </c>
-      <c r="T87" s="6" t="str">
-        <f t="shared" si="7"/>
-        <v>-1,1100011,1100012,-1,-1,-1</v>
-      </c>
-      <c r="U87" s="6">
-        <v>-1</v>
-      </c>
-      <c r="V87" s="6">
-        <v>1200</v>
-      </c>
-      <c r="W87" s="6">
-        <v>1201</v>
-      </c>
-      <c r="X87" s="6">
-        <v>1202</v>
-      </c>
-      <c r="Y87" s="6">
-        <v>1203</v>
-      </c>
-      <c r="Z87" s="6">
-        <v>1204</v>
-      </c>
-      <c r="AA87" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v>-1,1200,1201,1202,1203,1204</v>
-      </c>
-    </row>
-    <row r="88" customHeight="1" spans="3:27">
-      <c r="C88" s="6">
-        <v>1081</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E88" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="F88" s="1">
-        <v>3</v>
-      </c>
-      <c r="G88" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H88" s="1">
-        <v>2020</v>
-      </c>
-      <c r="I88" s="1">
-        <v>2021</v>
-      </c>
-      <c r="J88" s="1">
-        <v>2022</v>
-      </c>
-      <c r="K88" s="1">
-        <v>2023</v>
-      </c>
-      <c r="L88" s="1">
-        <v>2024</v>
-      </c>
-      <c r="M88" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>2020,2020,2021,2022,2023,2024</v>
-      </c>
-      <c r="N88" s="6">
-        <v>-1</v>
-      </c>
-      <c r="O88" s="6">
-        <v>1100011</v>
-      </c>
-      <c r="P88" s="6">
-        <v>1100012</v>
-      </c>
-      <c r="Q88" s="6">
-        <v>-1</v>
-      </c>
-      <c r="R88" s="6">
-        <v>-1</v>
-      </c>
-      <c r="S88" s="6">
-        <v>-1</v>
-      </c>
-      <c r="T88" s="6" t="str">
-        <f t="shared" si="7"/>
-        <v>-1,1100011,1100012,-1,-1,-1</v>
-      </c>
-      <c r="U88" s="6">
-        <v>-1</v>
-      </c>
-      <c r="V88" s="6">
-        <v>1200</v>
-      </c>
-      <c r="W88" s="6">
-        <v>1201</v>
-      </c>
-      <c r="X88" s="6">
-        <v>1202</v>
-      </c>
-      <c r="Y88" s="6">
-        <v>1203</v>
-      </c>
-      <c r="Z88" s="6">
-        <v>1204</v>
-      </c>
-      <c r="AA88" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v>-1,1200,1201,1202,1203,1204</v>
-      </c>
-    </row>
-    <row r="89" customHeight="1" spans="3:27">
-      <c r="C89" s="6">
-        <v>1082</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E89" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="F89" s="1">
-        <v>3</v>
-      </c>
-      <c r="G89" s="6">
-        <v>2010</v>
-      </c>
-      <c r="H89" s="6">
-        <v>2010</v>
-      </c>
-      <c r="I89" s="6">
-        <v>2011</v>
-      </c>
-      <c r="J89" s="6">
-        <v>2012</v>
-      </c>
-      <c r="K89" s="6">
-        <v>2013</v>
-      </c>
-      <c r="L89" s="6">
-        <v>2014</v>
-      </c>
-      <c r="M89" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>2010,2010,2011,2012,2013,2014</v>
-      </c>
-      <c r="N89" s="6">
-        <v>-1</v>
-      </c>
-      <c r="O89" s="6">
-        <v>1100011</v>
-      </c>
-      <c r="P89" s="6">
-        <v>1100012</v>
-      </c>
-      <c r="Q89" s="6">
-        <v>-1</v>
-      </c>
-      <c r="R89" s="6">
-        <v>-1</v>
-      </c>
-      <c r="S89" s="6">
-        <v>-1</v>
-      </c>
-      <c r="T89" s="6" t="str">
-        <f t="shared" si="7"/>
-        <v>-1,1100011,1100012,-1,-1,-1</v>
-      </c>
-      <c r="U89" s="6">
-        <v>-1</v>
-      </c>
-      <c r="V89" s="6">
-        <v>1200</v>
-      </c>
-      <c r="W89" s="6">
-        <v>1201</v>
-      </c>
-      <c r="X89" s="6">
-        <v>1202</v>
-      </c>
-      <c r="Y89" s="6">
-        <v>1203</v>
-      </c>
-      <c r="Z89" s="6">
-        <v>1204</v>
-      </c>
-      <c r="AA89" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v>-1,1200,1201,1202,1203,1204</v>
-      </c>
-    </row>
-    <row r="90" customHeight="1" spans="3:27">
-      <c r="C90" s="6">
-        <v>1083</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E90" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="F90" s="1">
-        <v>3</v>
-      </c>
-      <c r="G90" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H90" s="1">
-        <v>2020</v>
-      </c>
-      <c r="I90" s="1">
-        <v>2021</v>
-      </c>
-      <c r="J90" s="1">
-        <v>2022</v>
-      </c>
-      <c r="K90" s="1">
-        <v>2023</v>
-      </c>
-      <c r="L90" s="1">
-        <v>2024</v>
-      </c>
-      <c r="M90" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>2020,2020,2021,2022,2023,2024</v>
-      </c>
-      <c r="N90" s="6">
-        <v>-1</v>
-      </c>
-      <c r="O90" s="6">
-        <v>1100011</v>
-      </c>
-      <c r="P90" s="6">
-        <v>1100012</v>
-      </c>
-      <c r="Q90" s="6">
-        <v>-1</v>
-      </c>
-      <c r="R90" s="6">
-        <v>-1</v>
-      </c>
-      <c r="S90" s="6">
-        <v>-1</v>
-      </c>
-      <c r="T90" s="6" t="str">
-        <f t="shared" si="7"/>
-        <v>-1,1100011,1100012,-1,-1,-1</v>
-      </c>
-      <c r="U90" s="6">
-        <v>-1</v>
-      </c>
-      <c r="V90" s="6">
-        <v>1200</v>
-      </c>
-      <c r="W90" s="6">
-        <v>1201</v>
-      </c>
-      <c r="X90" s="6">
-        <v>1202</v>
-      </c>
-      <c r="Y90" s="6">
-        <v>1203</v>
-      </c>
-      <c r="Z90" s="6">
-        <v>1204</v>
-      </c>
-      <c r="AA90" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v>-1,1200,1201,1202,1203,1204</v>
-      </c>
-    </row>
-    <row r="91" customHeight="1" spans="3:27">
-      <c r="C91" s="6">
-        <v>1084</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E91" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="F91" s="1">
-        <v>3</v>
-      </c>
-      <c r="G91" s="6">
-        <v>2010</v>
-      </c>
-      <c r="H91" s="6">
-        <v>2010</v>
-      </c>
-      <c r="I91" s="6">
-        <v>2011</v>
-      </c>
-      <c r="J91" s="6">
-        <v>2012</v>
-      </c>
-      <c r="K91" s="6">
-        <v>2013</v>
-      </c>
-      <c r="L91" s="6">
-        <v>2014</v>
-      </c>
-      <c r="M91" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>2010,2010,2011,2012,2013,2014</v>
-      </c>
-      <c r="N91" s="6">
-        <v>-1</v>
-      </c>
-      <c r="O91" s="6">
-        <v>1100011</v>
-      </c>
-      <c r="P91" s="6">
-        <v>1100012</v>
-      </c>
-      <c r="Q91" s="6">
-        <v>-1</v>
-      </c>
-      <c r="R91" s="6">
-        <v>-1</v>
-      </c>
-      <c r="S91" s="6">
-        <v>-1</v>
-      </c>
-      <c r="T91" s="6" t="str">
-        <f t="shared" si="7"/>
-        <v>-1,1100011,1100012,-1,-1,-1</v>
-      </c>
-      <c r="U91" s="6">
-        <v>-1</v>
-      </c>
-      <c r="V91" s="6">
-        <v>1200</v>
-      </c>
-      <c r="W91" s="6">
-        <v>1201</v>
-      </c>
-      <c r="X91" s="6">
-        <v>1202</v>
-      </c>
-      <c r="Y91" s="6">
-        <v>1203</v>
-      </c>
-      <c r="Z91" s="6">
-        <v>1204</v>
-      </c>
-      <c r="AA91" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v>-1,1200,1201,1202,1203,1204</v>
-      </c>
-    </row>
-    <row r="92" customHeight="1" spans="3:27">
-      <c r="C92" s="6">
-        <v>1085</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E92" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="F92" s="1">
-        <v>3</v>
-      </c>
-      <c r="G92" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H92" s="1">
-        <v>2020</v>
-      </c>
-      <c r="I92" s="1">
-        <v>2021</v>
-      </c>
-      <c r="J92" s="1">
-        <v>2022</v>
-      </c>
-      <c r="K92" s="1">
-        <v>2023</v>
-      </c>
-      <c r="L92" s="1">
-        <v>2024</v>
-      </c>
-      <c r="M92" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>2020,2020,2021,2022,2023,2024</v>
-      </c>
-      <c r="N92" s="6">
-        <v>-1</v>
-      </c>
-      <c r="O92" s="6">
-        <v>1100011</v>
-      </c>
-      <c r="P92" s="6">
-        <v>1100012</v>
-      </c>
-      <c r="Q92" s="6">
-        <v>-1</v>
-      </c>
-      <c r="R92" s="6">
-        <v>-1</v>
-      </c>
-      <c r="S92" s="6">
-        <v>-1</v>
-      </c>
-      <c r="T92" s="6" t="str">
-        <f t="shared" si="7"/>
-        <v>-1,1100011,1100012,-1,-1,-1</v>
-      </c>
-      <c r="U92" s="6">
-        <v>-1</v>
-      </c>
-      <c r="V92" s="6">
-        <v>1200</v>
-      </c>
-      <c r="W92" s="6">
-        <v>1201</v>
-      </c>
-      <c r="X92" s="6">
-        <v>1202</v>
-      </c>
-      <c r="Y92" s="6">
-        <v>1203</v>
-      </c>
-      <c r="Z92" s="6">
-        <v>1204</v>
-      </c>
-      <c r="AA92" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v>-1,1200,1201,1202,1203,1204</v>
-      </c>
-    </row>
-    <row r="93" customHeight="1" spans="3:27">
-      <c r="C93" s="6">
-        <v>1086</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E93" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="F93" s="1">
-        <v>3</v>
-      </c>
-      <c r="G93" s="6">
-        <v>2010</v>
-      </c>
-      <c r="H93" s="6">
-        <v>2010</v>
-      </c>
-      <c r="I93" s="6">
-        <v>2011</v>
-      </c>
-      <c r="J93" s="6">
-        <v>2012</v>
-      </c>
-      <c r="K93" s="6">
-        <v>2013</v>
-      </c>
-      <c r="L93" s="6">
-        <v>2014</v>
-      </c>
-      <c r="M93" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>2010,2010,2011,2012,2013,2014</v>
-      </c>
-      <c r="N93" s="6">
-        <v>-1</v>
-      </c>
-      <c r="O93" s="6">
-        <v>1100011</v>
-      </c>
-      <c r="P93" s="6">
-        <v>1100012</v>
-      </c>
-      <c r="Q93" s="6">
-        <v>-1</v>
-      </c>
-      <c r="R93" s="6">
-        <v>-1</v>
-      </c>
-      <c r="S93" s="6">
-        <v>-1</v>
-      </c>
-      <c r="T93" s="6" t="str">
-        <f t="shared" si="7"/>
-        <v>-1,1100011,1100012,-1,-1,-1</v>
-      </c>
-      <c r="U93" s="6">
-        <v>-1</v>
-      </c>
-      <c r="V93" s="6">
-        <v>1200</v>
-      </c>
-      <c r="W93" s="6">
-        <v>1201</v>
-      </c>
-      <c r="X93" s="6">
-        <v>1202</v>
-      </c>
-      <c r="Y93" s="6">
-        <v>1203</v>
-      </c>
-      <c r="Z93" s="6">
-        <v>1204</v>
-      </c>
-      <c r="AA93" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v>-1,1200,1201,1202,1203,1204</v>
-      </c>
-    </row>
-    <row r="94" customHeight="1" spans="3:27">
-      <c r="C94" s="6">
-        <v>1087</v>
-      </c>
-      <c r="D94" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E94" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="F94" s="1">
-        <v>3</v>
-      </c>
-      <c r="G94" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H94" s="1">
-        <v>2020</v>
-      </c>
-      <c r="I94" s="1">
-        <v>2021</v>
-      </c>
-      <c r="J94" s="1">
-        <v>2022</v>
-      </c>
-      <c r="K94" s="1">
-        <v>2023</v>
-      </c>
-      <c r="L94" s="1">
-        <v>2024</v>
-      </c>
-      <c r="M94" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>2020,2020,2021,2022,2023,2024</v>
-      </c>
-      <c r="N94" s="6">
-        <v>-1</v>
-      </c>
-      <c r="O94" s="6">
-        <v>1100011</v>
-      </c>
-      <c r="P94" s="6">
-        <v>1100012</v>
-      </c>
-      <c r="Q94" s="6">
-        <v>-1</v>
-      </c>
-      <c r="R94" s="6">
-        <v>-1</v>
-      </c>
-      <c r="S94" s="6">
-        <v>-1</v>
-      </c>
-      <c r="T94" s="6" t="str">
-        <f t="shared" si="7"/>
-        <v>-1,1100011,1100012,-1,-1,-1</v>
-      </c>
-      <c r="U94" s="6">
-        <v>-1</v>
-      </c>
-      <c r="V94" s="6">
-        <v>1200</v>
-      </c>
-      <c r="W94" s="6">
-        <v>1201</v>
-      </c>
-      <c r="X94" s="6">
-        <v>1202</v>
-      </c>
-      <c r="Y94" s="6">
-        <v>1203</v>
-      </c>
-      <c r="Z94" s="6">
-        <v>1204</v>
-      </c>
-      <c r="AA94" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v>-1,1200,1201,1202,1203,1204</v>
-      </c>
-    </row>
-    <row r="95" customHeight="1" spans="3:27">
-      <c r="C95" s="6">
-        <v>1088</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E95" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="F95" s="1">
-        <v>3</v>
-      </c>
-      <c r="G95" s="6">
-        <v>2010</v>
-      </c>
-      <c r="H95" s="6">
-        <v>2010</v>
-      </c>
-      <c r="I95" s="6">
-        <v>2011</v>
-      </c>
-      <c r="J95" s="6">
-        <v>2012</v>
-      </c>
-      <c r="K95" s="6">
-        <v>2013</v>
-      </c>
-      <c r="L95" s="6">
-        <v>2014</v>
-      </c>
-      <c r="M95" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>2010,2010,2011,2012,2013,2014</v>
-      </c>
-      <c r="N95" s="6">
-        <v>-1</v>
-      </c>
-      <c r="O95" s="6">
-        <v>1100011</v>
-      </c>
-      <c r="P95" s="6">
-        <v>1100012</v>
-      </c>
-      <c r="Q95" s="6">
-        <v>-1</v>
-      </c>
-      <c r="R95" s="6">
-        <v>-1</v>
-      </c>
-      <c r="S95" s="6">
-        <v>-1</v>
-      </c>
-      <c r="T95" s="6" t="str">
-        <f t="shared" si="7"/>
-        <v>-1,1100011,1100012,-1,-1,-1</v>
-      </c>
-      <c r="U95" s="6">
-        <v>-1</v>
-      </c>
-      <c r="V95" s="6">
-        <v>1200</v>
-      </c>
-      <c r="W95" s="6">
-        <v>1201</v>
-      </c>
-      <c r="X95" s="6">
-        <v>1202</v>
-      </c>
-      <c r="Y95" s="6">
-        <v>1203</v>
-      </c>
-      <c r="Z95" s="6">
-        <v>1204</v>
-      </c>
-      <c r="AA95" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v>-1,1200,1201,1202,1203,1204</v>
-      </c>
-    </row>
-    <row r="96" customHeight="1" spans="3:27">
-      <c r="C96" s="6">
-        <v>1089</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E96" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="F96" s="1">
-        <v>3</v>
-      </c>
-      <c r="G96" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H96" s="1">
-        <v>2020</v>
-      </c>
-      <c r="I96" s="1">
-        <v>2021</v>
-      </c>
-      <c r="J96" s="1">
-        <v>2022</v>
-      </c>
-      <c r="K96" s="1">
-        <v>2023</v>
-      </c>
-      <c r="L96" s="1">
-        <v>2024</v>
-      </c>
-      <c r="M96" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>2020,2020,2021,2022,2023,2024</v>
-      </c>
-      <c r="N96" s="6">
-        <v>-1</v>
-      </c>
-      <c r="O96" s="6">
-        <v>1100011</v>
-      </c>
-      <c r="P96" s="6">
-        <v>1100012</v>
-      </c>
-      <c r="Q96" s="6">
-        <v>-1</v>
-      </c>
-      <c r="R96" s="6">
-        <v>-1</v>
-      </c>
-      <c r="S96" s="6">
-        <v>-1</v>
-      </c>
-      <c r="T96" s="6" t="str">
-        <f t="shared" si="7"/>
-        <v>-1,1100011,1100012,-1,-1,-1</v>
-      </c>
-      <c r="U96" s="6">
-        <v>-1</v>
-      </c>
-      <c r="V96" s="6">
-        <v>1200</v>
-      </c>
-      <c r="W96" s="6">
-        <v>1201</v>
-      </c>
-      <c r="X96" s="6">
-        <v>1202</v>
-      </c>
-      <c r="Y96" s="6">
-        <v>1203</v>
-      </c>
-      <c r="Z96" s="6">
-        <v>1204</v>
-      </c>
-      <c r="AA96" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v>-1,1200,1201,1202,1203,1204</v>
-      </c>
-    </row>
-    <row r="97" customHeight="1" spans="5:5">
-      <c r="E97" s="7"/>
-    </row>
-    <row r="98" customHeight="1" spans="5:5">
-      <c r="E98" s="7"/>
-    </row>
-    <row r="99" customHeight="1" spans="5:5">
-      <c r="E99" s="7"/>
-    </row>
-    <row r="100" customHeight="1" spans="5:5">
-      <c r="E100" s="7"/>
-    </row>
-    <row r="101" customHeight="1" spans="5:5">
-      <c r="E101" s="7"/>
+    <row r="71" customHeight="1" spans="5:5">
+      <c r="E71" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>